<commit_message>
Bugfix Bonn Produktuebersicht Raw
</commit_message>
<xml_diff>
--- a/Bonn/raw/ProduktuebersichtBonn2016.xlsx
+++ b/Bonn/raw/ProduktuebersichtBonn2016.xlsx
@@ -991,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G185"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,7 +1046,6 @@
         <v>8</v>
       </c>
       <c r="G2" s="4">
-        <f>C2*100</f>
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bug Fixes Bonn Code Lists
</commit_message>
<xml_diff>
--- a/Bonn/raw/ProduktuebersichtBonn2016.xlsx
+++ b/Bonn/raw/ProduktuebersichtBonn2016.xlsx
@@ -991,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G185"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="G165" sqref="G165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,9 +1045,7 @@
       <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="4">
-        <v>100</v>
-      </c>
+      <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -1827,9 +1825,7 @@
       <c r="F36" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G36" s="4">
-        <v>200</v>
-      </c>
+      <c r="G36" s="4"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
@@ -2172,9 +2168,7 @@
       <c r="F51" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G51" s="4">
-        <v>300</v>
-      </c>
+      <c r="G51" s="4"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
@@ -2425,9 +2419,7 @@
       <c r="F62" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G62" s="4">
-        <v>400</v>
-      </c>
+      <c r="G62" s="4"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
@@ -2770,9 +2762,7 @@
       <c r="F77" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G77" s="4">
-        <v>500</v>
-      </c>
+      <c r="G77" s="4"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
@@ -3092,9 +3082,7 @@
       <c r="F91" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G91" s="4">
-        <v>600</v>
-      </c>
+      <c r="G91" s="4"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
@@ -3299,9 +3287,7 @@
       <c r="F100" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G100" s="4">
-        <v>700</v>
-      </c>
+      <c r="G100" s="4"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
@@ -3414,9 +3400,7 @@
       <c r="F105" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="G105" s="4">
-        <v>800</v>
-      </c>
+      <c r="G105" s="4"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
@@ -3506,9 +3490,7 @@
       <c r="F109" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="G109" s="4">
-        <v>900</v>
-      </c>
+      <c r="G109" s="4"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
@@ -3759,9 +3741,7 @@
       <c r="F120" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="G120" s="4">
-        <v>1000</v>
-      </c>
+      <c r="G120" s="4"/>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
@@ -3897,9 +3877,7 @@
       <c r="F126" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="G126" s="4">
-        <v>1100</v>
-      </c>
+      <c r="G126" s="4"/>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
@@ -4012,9 +3990,7 @@
       <c r="F131" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="G131" s="4">
-        <v>1200</v>
-      </c>
+      <c r="G131" s="4"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
@@ -4219,9 +4195,7 @@
       <c r="F140" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="G140" s="4">
-        <v>1300</v>
-      </c>
+      <c r="G140" s="4"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
@@ -4357,9 +4331,7 @@
       <c r="F146" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="G146" s="4">
-        <v>1400</v>
-      </c>
+      <c r="G146" s="4"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
@@ -4426,9 +4398,7 @@
       <c r="F149" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G149" s="4">
-        <v>1500</v>
-      </c>
+      <c r="G149" s="4"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
@@ -4633,9 +4603,7 @@
       <c r="F158" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="G158" s="4">
-        <v>1600</v>
-      </c>
+      <c r="G158" s="4"/>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
@@ -4794,9 +4762,7 @@
       <c r="F165" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="G165" s="4">
-        <v>1700</v>
-      </c>
+      <c r="G165" s="4"/>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">

</xml_diff>

<commit_message>
Bug Fixes Bonn Code List
Produktübersicht (raw + transformed)
</commit_message>
<xml_diff>
--- a/Bonn/raw/ProduktuebersichtBonn2016.xlsx
+++ b/Bonn/raw/ProduktuebersichtBonn2016.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="203">
   <si>
     <t>Produktbereich</t>
   </si>
@@ -165,9 +165,6 @@
   </si>
   <si>
     <t>Wahlen</t>
-  </si>
-  <si>
-    <t>Amt 37 TE-übergreifend</t>
   </si>
   <si>
     <t>Brandschutz</t>
@@ -989,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G185"/>
+  <dimension ref="A1:G184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="G165" sqref="G165"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1993,16 +1990,16 @@
         <v>38</v>
       </c>
       <c r="B44" s="2">
-        <v>137000200</v>
+        <v>137000219</v>
       </c>
       <c r="C44" s="3">
         <v>2</v>
       </c>
       <c r="D44" s="3">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="E44" s="4">
-        <v>200</v>
+        <v>219</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>47</v>
@@ -2016,16 +2013,16 @@
         <v>38</v>
       </c>
       <c r="B45" s="2">
-        <v>137000219</v>
+        <v>137000220</v>
       </c>
       <c r="C45" s="3">
         <v>2</v>
       </c>
       <c r="D45" s="3">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E45" s="4">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>48</v>
@@ -2039,16 +2036,16 @@
         <v>38</v>
       </c>
       <c r="B46" s="2">
-        <v>137000220</v>
+        <v>137000221</v>
       </c>
       <c r="C46" s="3">
         <v>2</v>
       </c>
       <c r="D46" s="3">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E46" s="4">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>49</v>
@@ -2062,16 +2059,16 @@
         <v>38</v>
       </c>
       <c r="B47" s="2">
-        <v>137000221</v>
+        <v>156000208</v>
       </c>
       <c r="C47" s="3">
         <v>2</v>
       </c>
       <c r="D47" s="3">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E47" s="4">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>50</v>
@@ -2085,16 +2082,16 @@
         <v>38</v>
       </c>
       <c r="B48" s="2">
-        <v>156000208</v>
+        <v>156000209</v>
       </c>
       <c r="C48" s="3">
         <v>2</v>
       </c>
       <c r="D48" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E48" s="4">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>51</v>
@@ -2108,16 +2105,16 @@
         <v>38</v>
       </c>
       <c r="B49" s="2">
-        <v>156000209</v>
+        <v>161000215</v>
       </c>
       <c r="C49" s="3">
         <v>2</v>
       </c>
       <c r="D49" s="3">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E49" s="4">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>52</v>
@@ -2128,63 +2125,63 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B50" s="2">
-        <v>161000215</v>
+        <v>140000300</v>
       </c>
       <c r="C50" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D50" s="3">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E50" s="4">
-        <v>215</v>
+        <v>300</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G50" s="4">
-        <v>200</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="G50" s="4"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B51" s="2">
-        <v>140000300</v>
+        <v>140000301</v>
       </c>
       <c r="C51" s="3">
         <v>3</v>
       </c>
       <c r="D51" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E51" s="4">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G51" s="4"/>
+      <c r="G51" s="4">
+        <v>300</v>
+      </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B52" s="2">
-        <v>140000301</v>
+        <v>140000302</v>
       </c>
       <c r="C52" s="3">
         <v>3</v>
       </c>
       <c r="D52" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E52" s="4">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>56</v>
@@ -2195,19 +2192,19 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B53" s="2">
-        <v>140000302</v>
+        <v>140000303</v>
       </c>
       <c r="C53" s="3">
         <v>3</v>
       </c>
       <c r="D53" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E53" s="4">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>57</v>
@@ -2218,19 +2215,19 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B54" s="2">
-        <v>140000303</v>
+        <v>140000304</v>
       </c>
       <c r="C54" s="3">
         <v>3</v>
       </c>
       <c r="D54" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E54" s="4">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>58</v>
@@ -2241,19 +2238,19 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55" s="2">
-        <v>140000304</v>
+        <v>140000305</v>
       </c>
       <c r="C55" s="3">
         <v>3</v>
       </c>
       <c r="D55" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E55" s="4">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>59</v>
@@ -2264,19 +2261,19 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56" s="2">
-        <v>140000305</v>
+        <v>140000306</v>
       </c>
       <c r="C56" s="3">
         <v>3</v>
       </c>
       <c r="D56" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E56" s="4">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>60</v>
@@ -2287,19 +2284,19 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B57" s="2">
-        <v>140000306</v>
+        <v>140000307</v>
       </c>
       <c r="C57" s="3">
         <v>3</v>
       </c>
       <c r="D57" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E57" s="4">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>61</v>
@@ -2310,19 +2307,19 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B58" s="2">
-        <v>140000307</v>
+        <v>140000308</v>
       </c>
       <c r="C58" s="3">
         <v>3</v>
       </c>
       <c r="D58" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E58" s="4">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>62</v>
@@ -2333,19 +2330,19 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B59" s="2">
-        <v>140000308</v>
+        <v>140000309</v>
       </c>
       <c r="C59" s="3">
         <v>3</v>
       </c>
       <c r="D59" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E59" s="4">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>63</v>
@@ -2356,19 +2353,19 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B60" s="2">
-        <v>140000309</v>
+        <v>140000310</v>
       </c>
       <c r="C60" s="3">
         <v>3</v>
       </c>
       <c r="D60" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E60" s="4">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>64</v>
@@ -2379,63 +2376,63 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="B61" s="2">
-        <v>140000310</v>
+        <v>100000400</v>
       </c>
       <c r="C61" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D61" s="3">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E61" s="4">
-        <v>310</v>
+        <v>400</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G61" s="4">
-        <v>300</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="G61" s="4"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B62" s="2">
-        <v>100000400</v>
+        <v>141000401</v>
       </c>
       <c r="C62" s="3">
         <v>4</v>
       </c>
       <c r="D62" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62" s="4">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G62" s="4"/>
+      <c r="G62" s="4">
+        <v>400</v>
+      </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B63" s="2">
-        <v>141000401</v>
+        <v>141000402</v>
       </c>
       <c r="C63" s="3">
         <v>4</v>
       </c>
       <c r="D63" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E63" s="4">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>68</v>
@@ -2446,19 +2443,19 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B64" s="2">
-        <v>141000402</v>
+        <v>141000403</v>
       </c>
       <c r="C64" s="3">
         <v>4</v>
       </c>
       <c r="D64" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E64" s="4">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>69</v>
@@ -2469,19 +2466,19 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B65" s="2">
-        <v>141000403</v>
+        <v>141200410</v>
       </c>
       <c r="C65" s="3">
         <v>4</v>
       </c>
       <c r="D65" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E65" s="4">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>70</v>
@@ -2492,19 +2489,19 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B66" s="2">
-        <v>141200410</v>
+        <v>141300409</v>
       </c>
       <c r="C66" s="3">
         <v>4</v>
       </c>
       <c r="D66" s="3">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E66" s="4">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>71</v>
@@ -2515,19 +2512,19 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B67" s="2">
-        <v>141300409</v>
+        <v>141400407</v>
       </c>
       <c r="C67" s="3">
         <v>4</v>
       </c>
       <c r="D67" s="3">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E67" s="4">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>72</v>
@@ -2538,19 +2535,19 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B68" s="2">
-        <v>141400407</v>
+        <v>141500408</v>
       </c>
       <c r="C68" s="3">
         <v>4</v>
       </c>
       <c r="D68" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E68" s="4">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>73</v>
@@ -2561,19 +2558,19 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B69" s="2">
-        <v>141500408</v>
+        <v>141600406</v>
       </c>
       <c r="C69" s="3">
         <v>4</v>
       </c>
       <c r="D69" s="3">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E69" s="4">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>74</v>
@@ -2584,19 +2581,19 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B70" s="2">
-        <v>141600406</v>
+        <v>141700405</v>
       </c>
       <c r="C70" s="3">
         <v>4</v>
       </c>
       <c r="D70" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E70" s="4">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>75</v>
@@ -2607,19 +2604,19 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B71" s="2">
-        <v>141700405</v>
+        <v>141800404</v>
       </c>
       <c r="C71" s="3">
         <v>4</v>
       </c>
       <c r="D71" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E71" s="4">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>76</v>
@@ -2630,19 +2627,19 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B72" s="2">
-        <v>141800404</v>
+        <v>141900411</v>
       </c>
       <c r="C72" s="3">
         <v>4</v>
       </c>
       <c r="D72" s="3">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E72" s="4">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>77</v>
@@ -2653,19 +2650,19 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B73" s="2">
-        <v>141900411</v>
+        <v>190000414</v>
       </c>
       <c r="C73" s="3">
         <v>4</v>
       </c>
       <c r="D73" s="3">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E73" s="4">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>78</v>
@@ -2676,19 +2673,19 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B74" s="2">
-        <v>190000414</v>
+        <v>190400412</v>
       </c>
       <c r="C74" s="3">
         <v>4</v>
       </c>
       <c r="D74" s="3">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E74" s="4">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>79</v>
@@ -2699,19 +2696,19 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B75" s="2">
-        <v>190400412</v>
+        <v>190400413</v>
       </c>
       <c r="C75" s="3">
         <v>4</v>
       </c>
       <c r="D75" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E75" s="4">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>80</v>
@@ -2722,63 +2719,63 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B76" s="2">
-        <v>190400413</v>
+        <v>100000500</v>
       </c>
       <c r="C76" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D76" s="3">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E76" s="4">
-        <v>413</v>
+        <v>500</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="G76" s="4">
-        <v>400</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="G76" s="4"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B77" s="2">
-        <v>100000500</v>
+        <v>130000512</v>
       </c>
       <c r="C77" s="3">
         <v>5</v>
       </c>
       <c r="D77" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E77" s="4">
-        <v>500</v>
+        <v>512</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="G77" s="4"/>
+      <c r="G77" s="4">
+        <v>500</v>
+      </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B78" s="2">
-        <v>130000512</v>
+        <v>130000513</v>
       </c>
       <c r="C78" s="3">
         <v>5</v>
       </c>
       <c r="D78" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E78" s="4">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>84</v>
@@ -2789,19 +2786,19 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B79" s="2">
-        <v>130000513</v>
+        <v>150000501</v>
       </c>
       <c r="C79" s="3">
         <v>5</v>
       </c>
       <c r="D79" s="3">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E79" s="4">
-        <v>513</v>
+        <v>501</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>85</v>
@@ -2812,19 +2809,19 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B80" s="2">
-        <v>150000501</v>
+        <v>150000502</v>
       </c>
       <c r="C80" s="3">
         <v>5</v>
       </c>
       <c r="D80" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E80" s="4">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>86</v>
@@ -2835,19 +2832,19 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B81" s="2">
-        <v>150000502</v>
+        <v>150000503</v>
       </c>
       <c r="C81" s="3">
         <v>5</v>
       </c>
       <c r="D81" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E81" s="4">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>87</v>
@@ -2858,19 +2855,19 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B82" s="2">
-        <v>150000503</v>
+        <v>150000504</v>
       </c>
       <c r="C82" s="3">
         <v>5</v>
       </c>
       <c r="D82" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E82" s="4">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>88</v>
@@ -2881,19 +2878,19 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B83" s="2">
-        <v>150000504</v>
+        <v>150000505</v>
       </c>
       <c r="C83" s="3">
         <v>5</v>
       </c>
       <c r="D83" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E83" s="4">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>89</v>
@@ -2904,19 +2901,19 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B84" s="2">
-        <v>150000505</v>
+        <v>150000506</v>
       </c>
       <c r="C84" s="3">
         <v>5</v>
       </c>
       <c r="D84" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E84" s="4">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>90</v>
@@ -2927,19 +2924,19 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B85" s="2">
-        <v>150000506</v>
+        <v>150000507</v>
       </c>
       <c r="C85" s="3">
         <v>5</v>
       </c>
       <c r="D85" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E85" s="4">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>91</v>
@@ -2950,19 +2947,19 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B86" s="2">
-        <v>150000507</v>
+        <v>150000508</v>
       </c>
       <c r="C86" s="3">
         <v>5</v>
       </c>
       <c r="D86" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E86" s="4">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>92</v>
@@ -2973,19 +2970,19 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B87" s="2">
-        <v>150000508</v>
+        <v>150000509</v>
       </c>
       <c r="C87" s="3">
         <v>5</v>
       </c>
       <c r="D87" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E87" s="4">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>93</v>
@@ -2996,19 +2993,19 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B88" s="2">
-        <v>150000509</v>
+        <v>150000510</v>
       </c>
       <c r="C88" s="3">
         <v>5</v>
       </c>
       <c r="D88" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E88" s="4">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>94</v>
@@ -3019,19 +3016,19 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B89" s="2">
-        <v>150000510</v>
+        <v>150000511</v>
       </c>
       <c r="C89" s="3">
         <v>5</v>
       </c>
       <c r="D89" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E89" s="4">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>95</v>
@@ -3042,63 +3039,63 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="B90" s="2">
-        <v>150000511</v>
+        <v>100000600</v>
       </c>
       <c r="C90" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D90" s="3">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E90" s="4">
-        <v>511</v>
+        <v>600</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G90" s="4">
-        <v>500</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="G90" s="4"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B91" s="2">
-        <v>100000600</v>
+        <v>150000607</v>
       </c>
       <c r="C91" s="3">
         <v>6</v>
       </c>
       <c r="D91" s="3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E91" s="4">
-        <v>600</v>
+        <v>607</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G91" s="4"/>
+      <c r="G91" s="4">
+        <v>600</v>
+      </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B92" s="2">
-        <v>150000607</v>
+        <v>151000601</v>
       </c>
       <c r="C92" s="3">
         <v>6</v>
       </c>
       <c r="D92" s="3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E92" s="4">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="F92" s="2" t="s">
         <v>99</v>
@@ -3109,19 +3106,19 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B93" s="2">
-        <v>151000601</v>
+        <v>151000602</v>
       </c>
       <c r="C93" s="3">
         <v>6</v>
       </c>
       <c r="D93" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E93" s="4">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>100</v>
@@ -3132,19 +3129,19 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B94" s="2">
-        <v>151000602</v>
+        <v>151000603</v>
       </c>
       <c r="C94" s="3">
         <v>6</v>
       </c>
       <c r="D94" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E94" s="4">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>101</v>
@@ -3155,19 +3152,19 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B95" s="2">
-        <v>151000603</v>
+        <v>151000604</v>
       </c>
       <c r="C95" s="3">
         <v>6</v>
       </c>
       <c r="D95" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E95" s="4">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>102</v>
@@ -3178,19 +3175,19 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B96" s="2">
-        <v>151000604</v>
+        <v>151000605</v>
       </c>
       <c r="C96" s="3">
         <v>6</v>
       </c>
       <c r="D96" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E96" s="4">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>103</v>
@@ -3201,19 +3198,19 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B97" s="2">
-        <v>151000605</v>
+        <v>151000606</v>
       </c>
       <c r="C97" s="3">
         <v>6</v>
       </c>
       <c r="D97" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E97" s="4">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>104</v>
@@ -3224,19 +3221,19 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B98" s="2">
-        <v>151000606</v>
+        <v>151000608</v>
       </c>
       <c r="C98" s="3">
         <v>6</v>
       </c>
       <c r="D98" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E98" s="4">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="F98" s="2" t="s">
         <v>105</v>
@@ -3247,63 +3244,63 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="B99" s="2">
-        <v>151000608</v>
+        <v>100000700</v>
       </c>
       <c r="C99" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D99" s="3">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E99" s="4">
-        <v>608</v>
+        <v>700</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G99" s="4">
-        <v>600</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="G99" s="4"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B100" s="2">
-        <v>100000700</v>
+        <v>153000701</v>
       </c>
       <c r="C100" s="3">
         <v>7</v>
       </c>
       <c r="D100" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E100" s="4">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="F100" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G100" s="4"/>
+      <c r="G100" s="4">
+        <v>700</v>
+      </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B101" s="2">
-        <v>153000701</v>
+        <v>153000702</v>
       </c>
       <c r="C101" s="3">
         <v>7</v>
       </c>
       <c r="D101" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E101" s="4">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="F101" s="2" t="s">
         <v>109</v>
@@ -3314,19 +3311,19 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B102" s="2">
-        <v>153000702</v>
+        <v>153000703</v>
       </c>
       <c r="C102" s="3">
         <v>7</v>
       </c>
       <c r="D102" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E102" s="4">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="F102" s="2" t="s">
         <v>110</v>
@@ -3337,19 +3334,19 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B103" s="2">
-        <v>153000703</v>
+        <v>153000704</v>
       </c>
       <c r="C103" s="3">
         <v>7</v>
       </c>
       <c r="D103" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E103" s="4">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="F103" s="2" t="s">
         <v>111</v>
@@ -3360,63 +3357,63 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B104" s="2">
-        <v>153000704</v>
+        <v>152000800</v>
       </c>
       <c r="C104" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D104" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E104" s="4">
-        <v>704</v>
+        <v>800</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G104" s="4">
-        <v>700</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="G104" s="4"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B105" s="2">
-        <v>152000800</v>
+        <v>152000801</v>
       </c>
       <c r="C105" s="3">
         <v>8</v>
       </c>
       <c r="D105" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E105" s="4">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="F105" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="G105" s="4"/>
+      <c r="G105" s="4">
+        <v>800</v>
+      </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B106" s="2">
-        <v>152000801</v>
+        <v>152000802</v>
       </c>
       <c r="C106" s="3">
         <v>8</v>
       </c>
       <c r="D106" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E106" s="4">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="F106" s="2" t="s">
         <v>115</v>
@@ -3427,19 +3424,19 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B107" s="2">
-        <v>152000802</v>
+        <v>152000803</v>
       </c>
       <c r="C107" s="3">
         <v>8</v>
       </c>
       <c r="D107" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E107" s="4">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="F107" s="2" t="s">
         <v>116</v>
@@ -3450,63 +3447,63 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B108" s="2">
-        <v>152000803</v>
+        <v>100000900</v>
       </c>
       <c r="C108" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D108" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E108" s="4">
-        <v>803</v>
+        <v>900</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G108" s="4">
-        <v>800</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="G108" s="4"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B109" s="2">
-        <v>100000900</v>
+        <v>123000905</v>
       </c>
       <c r="C109" s="3">
         <v>9</v>
       </c>
       <c r="D109" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E109" s="4">
-        <v>900</v>
+        <v>905</v>
       </c>
       <c r="F109" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="G109" s="4"/>
+      <c r="G109" s="4">
+        <v>900</v>
+      </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B110" s="2">
-        <v>123000905</v>
+        <v>125000910</v>
       </c>
       <c r="C110" s="3">
         <v>9</v>
       </c>
       <c r="D110" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E110" s="4">
-        <v>905</v>
+        <v>910</v>
       </c>
       <c r="F110" s="2" t="s">
         <v>120</v>
@@ -3517,19 +3514,19 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B111" s="2">
-        <v>125000910</v>
+        <v>161000901</v>
       </c>
       <c r="C111" s="3">
         <v>9</v>
       </c>
       <c r="D111" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E111" s="4">
-        <v>910</v>
+        <v>901</v>
       </c>
       <c r="F111" s="2" t="s">
         <v>121</v>
@@ -3540,19 +3537,19 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B112" s="2">
-        <v>161000901</v>
+        <v>161000902</v>
       </c>
       <c r="C112" s="3">
         <v>9</v>
       </c>
       <c r="D112" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E112" s="4">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="F112" s="2" t="s">
         <v>122</v>
@@ -3563,19 +3560,19 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B113" s="2">
-        <v>161000902</v>
+        <v>162000906</v>
       </c>
       <c r="C113" s="3">
         <v>9</v>
       </c>
       <c r="D113" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E113" s="4">
-        <v>902</v>
+        <v>906</v>
       </c>
       <c r="F113" s="2" t="s">
         <v>123</v>
@@ -3586,19 +3583,19 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B114" s="2">
-        <v>162000906</v>
+        <v>162000907</v>
       </c>
       <c r="C114" s="3">
         <v>9</v>
       </c>
       <c r="D114" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E114" s="4">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="F114" s="2" t="s">
         <v>124</v>
@@ -3609,19 +3606,19 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B115" s="2">
-        <v>162000907</v>
+        <v>162000908</v>
       </c>
       <c r="C115" s="3">
         <v>9</v>
       </c>
       <c r="D115" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E115" s="4">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="F115" s="2" t="s">
         <v>125</v>
@@ -3632,19 +3629,19 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B116" s="2">
-        <v>162000908</v>
+        <v>162000909</v>
       </c>
       <c r="C116" s="3">
         <v>9</v>
       </c>
       <c r="D116" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E116" s="4">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="F116" s="2" t="s">
         <v>126</v>
@@ -3655,19 +3652,19 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B117" s="2">
-        <v>162000909</v>
+        <v>163000904</v>
       </c>
       <c r="C117" s="3">
         <v>9</v>
       </c>
       <c r="D117" s="3">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E117" s="4">
-        <v>909</v>
+        <v>904</v>
       </c>
       <c r="F117" s="2" t="s">
         <v>127</v>
@@ -3678,19 +3675,19 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B118" s="2">
-        <v>163000904</v>
+        <v>190600903</v>
       </c>
       <c r="C118" s="3">
         <v>9</v>
       </c>
       <c r="D118" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E118" s="4">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="F118" s="2" t="s">
         <v>128</v>
@@ -3701,63 +3698,63 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="B119" s="2">
-        <v>190600903</v>
+        <v>100001000</v>
       </c>
       <c r="C119" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D119" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E119" s="4">
-        <v>903</v>
+        <v>1000</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G119" s="4">
-        <v>900</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="G119" s="4"/>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B120" s="2">
-        <v>100001000</v>
+        <v>120201006</v>
       </c>
       <c r="C120" s="3">
         <v>10</v>
       </c>
       <c r="D120" s="3">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E120" s="4">
-        <v>1000</v>
+        <v>1006</v>
       </c>
       <c r="F120" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="G120" s="4"/>
+      <c r="G120" s="4">
+        <v>1000</v>
+      </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B121" s="2">
-        <v>120201006</v>
+        <v>123001004</v>
       </c>
       <c r="C121" s="3">
         <v>10</v>
       </c>
       <c r="D121" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E121" s="4">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="F121" s="2" t="s">
         <v>132</v>
@@ -3768,19 +3765,19 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B122" s="2">
-        <v>123001004</v>
+        <v>150001005</v>
       </c>
       <c r="C122" s="3">
         <v>10</v>
       </c>
       <c r="D122" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E122" s="4">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="F122" s="2" t="s">
         <v>133</v>
@@ -3791,19 +3788,19 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B123" s="2">
-        <v>150001005</v>
+        <v>161001003</v>
       </c>
       <c r="C123" s="3">
         <v>10</v>
       </c>
       <c r="D123" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E123" s="4">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="F123" s="2" t="s">
         <v>134</v>
@@ -3814,19 +3811,19 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B124" s="2">
-        <v>161001003</v>
+        <v>163001001</v>
       </c>
       <c r="C124" s="3">
         <v>10</v>
       </c>
       <c r="D124" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E124" s="4">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="F124" s="2" t="s">
         <v>135</v>
@@ -3837,63 +3834,63 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="B125" s="2">
-        <v>163001001</v>
+        <v>100001100</v>
       </c>
       <c r="C125" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D125" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E125" s="4">
-        <v>1001</v>
+        <v>1100</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="G125" s="4">
-        <v>1000</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="G125" s="4"/>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B126" s="2">
-        <v>100001100</v>
+        <v>120201101</v>
       </c>
       <c r="C126" s="3">
         <v>11</v>
       </c>
       <c r="D126" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E126" s="4">
-        <v>1100</v>
+        <v>1101</v>
       </c>
       <c r="F126" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="G126" s="4"/>
+      <c r="G126" s="4">
+        <v>1100</v>
+      </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B127" s="2">
-        <v>120201101</v>
+        <v>166001103</v>
       </c>
       <c r="C127" s="3">
         <v>11</v>
       </c>
       <c r="D127" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E127" s="4">
-        <v>1101</v>
+        <v>1103</v>
       </c>
       <c r="F127" s="2" t="s">
         <v>139</v>
@@ -3904,19 +3901,19 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B128" s="2">
-        <v>166001103</v>
+        <v>170001102</v>
       </c>
       <c r="C128" s="3">
         <v>11</v>
       </c>
       <c r="D128" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E128" s="4">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="F128" s="2" t="s">
         <v>140</v>
@@ -3927,19 +3924,19 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B129" s="2">
-        <v>170001102</v>
+        <v>170001104</v>
       </c>
       <c r="C129" s="3">
         <v>11</v>
       </c>
       <c r="D129" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E129" s="4">
-        <v>1102</v>
+        <v>1104</v>
       </c>
       <c r="F129" s="2" t="s">
         <v>141</v>
@@ -3950,63 +3947,63 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="B130" s="2">
-        <v>170001104</v>
+        <v>100001200</v>
       </c>
       <c r="C130" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D130" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E130" s="4">
-        <v>1104</v>
+        <v>1200</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G130" s="4">
-        <v>1100</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="G130" s="4"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B131" s="2">
-        <v>100001200</v>
+        <v>161001207</v>
       </c>
       <c r="C131" s="3">
         <v>12</v>
       </c>
       <c r="D131" s="3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E131" s="4">
-        <v>1200</v>
+        <v>1207</v>
       </c>
       <c r="F131" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="G131" s="4"/>
+      <c r="G131" s="4">
+        <v>1200</v>
+      </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B132" s="2">
-        <v>161001207</v>
+        <v>166001201</v>
       </c>
       <c r="C132" s="3">
         <v>12</v>
       </c>
       <c r="D132" s="3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E132" s="4">
-        <v>1207</v>
+        <v>1201</v>
       </c>
       <c r="F132" s="2" t="s">
         <v>145</v>
@@ -4017,19 +4014,19 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B133" s="2">
-        <v>166001201</v>
+        <v>166001202</v>
       </c>
       <c r="C133" s="3">
         <v>12</v>
       </c>
       <c r="D133" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E133" s="4">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="F133" s="2" t="s">
         <v>146</v>
@@ -4040,19 +4037,19 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B134" s="2">
-        <v>166001202</v>
+        <v>166001203</v>
       </c>
       <c r="C134" s="3">
         <v>12</v>
       </c>
       <c r="D134" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E134" s="4">
-        <v>1202</v>
+        <v>1203</v>
       </c>
       <c r="F134" s="2" t="s">
         <v>147</v>
@@ -4063,19 +4060,19 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B135" s="2">
-        <v>166001203</v>
+        <v>166001204</v>
       </c>
       <c r="C135" s="3">
         <v>12</v>
       </c>
       <c r="D135" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E135" s="4">
-        <v>1203</v>
+        <v>1204</v>
       </c>
       <c r="F135" s="2" t="s">
         <v>148</v>
@@ -4086,19 +4083,19 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B136" s="2">
-        <v>166001204</v>
+        <v>166001205</v>
       </c>
       <c r="C136" s="3">
         <v>12</v>
       </c>
       <c r="D136" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E136" s="4">
-        <v>1204</v>
+        <v>1205</v>
       </c>
       <c r="F136" s="2" t="s">
         <v>149</v>
@@ -4109,19 +4106,19 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B137" s="2">
-        <v>166001205</v>
+        <v>166001206</v>
       </c>
       <c r="C137" s="3">
         <v>12</v>
       </c>
       <c r="D137" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E137" s="4">
-        <v>1205</v>
+        <v>1206</v>
       </c>
       <c r="F137" s="2" t="s">
         <v>150</v>
@@ -4132,19 +4129,19 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B138" s="2">
-        <v>166001206</v>
+        <v>170001208</v>
       </c>
       <c r="C138" s="3">
         <v>12</v>
       </c>
       <c r="D138" s="3">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E138" s="4">
-        <v>1206</v>
+        <v>1208</v>
       </c>
       <c r="F138" s="2" t="s">
         <v>151</v>
@@ -4155,63 +4152,63 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="B139" s="2">
-        <v>170001208</v>
+        <v>100001300</v>
       </c>
       <c r="C139" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D139" s="3">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E139" s="4">
-        <v>1208</v>
+        <v>1300</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="G139" s="4">
-        <v>1200</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="G139" s="4"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B140" s="2">
-        <v>100001300</v>
+        <v>156001307</v>
       </c>
       <c r="C140" s="3">
         <v>13</v>
       </c>
       <c r="D140" s="3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E140" s="4">
-        <v>1300</v>
+        <v>1307</v>
       </c>
       <c r="F140" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="G140" s="4"/>
+      <c r="G140" s="4">
+        <v>1300</v>
+      </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B141" s="2">
-        <v>156001307</v>
+        <v>166001308</v>
       </c>
       <c r="C141" s="3">
         <v>13</v>
       </c>
       <c r="D141" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E141" s="4">
-        <v>1307</v>
+        <v>1308</v>
       </c>
       <c r="F141" s="2" t="s">
         <v>155</v>
@@ -4222,19 +4219,19 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B142" s="2">
-        <v>166001308</v>
+        <v>168001301</v>
       </c>
       <c r="C142" s="3">
         <v>13</v>
       </c>
       <c r="D142" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E142" s="4">
-        <v>1308</v>
+        <v>1301</v>
       </c>
       <c r="F142" s="2" t="s">
         <v>156</v>
@@ -4245,19 +4242,19 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B143" s="2">
-        <v>168001301</v>
+        <v>168001302</v>
       </c>
       <c r="C143" s="3">
         <v>13</v>
       </c>
       <c r="D143" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E143" s="4">
-        <v>1301</v>
+        <v>1302</v>
       </c>
       <c r="F143" s="2" t="s">
         <v>157</v>
@@ -4268,19 +4265,19 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B144" s="2">
-        <v>168001302</v>
+        <v>168001303</v>
       </c>
       <c r="C144" s="3">
         <v>13</v>
       </c>
       <c r="D144" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E144" s="4">
-        <v>1302</v>
+        <v>1303</v>
       </c>
       <c r="F144" s="2" t="s">
         <v>158</v>
@@ -4291,63 +4288,63 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="B145" s="2">
-        <v>168001303</v>
+        <v>100001400</v>
       </c>
       <c r="C145" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D145" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E145" s="4">
-        <v>1303</v>
+        <v>1400</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="G145" s="4">
-        <v>1300</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="G145" s="4"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B146" s="2">
-        <v>100001400</v>
+        <v>156001401</v>
       </c>
       <c r="C146" s="3">
         <v>14</v>
       </c>
       <c r="D146" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E146" s="4">
-        <v>1400</v>
+        <v>1401</v>
       </c>
       <c r="F146" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="G146" s="4"/>
+      <c r="G146" s="4">
+        <v>1400</v>
+      </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B147" s="2">
-        <v>156001401</v>
+        <v>156001402</v>
       </c>
       <c r="C147" s="3">
         <v>14</v>
       </c>
       <c r="D147" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E147" s="4">
-        <v>1401</v>
+        <v>1402</v>
       </c>
       <c r="F147" s="2" t="s">
         <v>162</v>
@@ -4358,63 +4355,63 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B148" s="2">
-        <v>156001402</v>
+        <v>100001500</v>
       </c>
       <c r="C148" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D148" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E148" s="4">
-        <v>1402</v>
+        <v>1500</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="G148" s="4">
-        <v>1400</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="G148" s="4"/>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B149" s="2">
-        <v>100001500</v>
+        <v>103001501</v>
       </c>
       <c r="C149" s="3">
         <v>15</v>
       </c>
       <c r="D149" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E149" s="4">
-        <v>1500</v>
+        <v>1501</v>
       </c>
       <c r="F149" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="G149" s="4"/>
+      <c r="G149" s="4">
+        <v>1500</v>
+      </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B150" s="2">
-        <v>103001501</v>
+        <v>103001502</v>
       </c>
       <c r="C150" s="3">
         <v>15</v>
       </c>
       <c r="D150" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E150" s="4">
-        <v>1501</v>
+        <v>1502</v>
       </c>
       <c r="F150" s="2" t="s">
         <v>166</v>
@@ -4425,19 +4422,19 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B151" s="2">
-        <v>103001502</v>
+        <v>103001503</v>
       </c>
       <c r="C151" s="3">
         <v>15</v>
       </c>
       <c r="D151" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E151" s="4">
-        <v>1502</v>
+        <v>1503</v>
       </c>
       <c r="F151" s="2" t="s">
         <v>167</v>
@@ -4448,19 +4445,19 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B152" s="2">
-        <v>103001503</v>
+        <v>120001505</v>
       </c>
       <c r="C152" s="3">
         <v>15</v>
       </c>
       <c r="D152" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E152" s="4">
-        <v>1503</v>
+        <v>1505</v>
       </c>
       <c r="F152" s="2" t="s">
         <v>168</v>
@@ -4471,19 +4468,19 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B153" s="2">
-        <v>120001505</v>
+        <v>120201510</v>
       </c>
       <c r="C153" s="3">
         <v>15</v>
       </c>
       <c r="D153" s="3">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E153" s="4">
-        <v>1505</v>
+        <v>1510</v>
       </c>
       <c r="F153" s="2" t="s">
         <v>169</v>
@@ -4494,19 +4491,19 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B154" s="2">
-        <v>120201510</v>
+        <v>123001506</v>
       </c>
       <c r="C154" s="3">
         <v>15</v>
       </c>
       <c r="D154" s="3">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E154" s="4">
-        <v>1510</v>
+        <v>1506</v>
       </c>
       <c r="F154" s="2" t="s">
         <v>170</v>
@@ -4517,19 +4514,19 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B155" s="2">
-        <v>123001506</v>
+        <v>190001504</v>
       </c>
       <c r="C155" s="3">
         <v>15</v>
       </c>
       <c r="D155" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E155" s="4">
-        <v>1506</v>
+        <v>1504</v>
       </c>
       <c r="F155" s="2" t="s">
         <v>171</v>
@@ -4540,19 +4537,19 @@
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B156" s="2">
-        <v>190001504</v>
+        <v>190001507</v>
       </c>
       <c r="C156" s="3">
         <v>15</v>
       </c>
       <c r="D156" s="3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E156" s="4">
-        <v>1504</v>
+        <v>1507</v>
       </c>
       <c r="F156" s="2" t="s">
         <v>172</v>
@@ -4563,63 +4560,63 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="B157" s="2">
-        <v>190001507</v>
+        <v>100001600</v>
       </c>
       <c r="C157" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D157" s="3">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E157" s="4">
-        <v>1507</v>
+        <v>1600</v>
       </c>
       <c r="F157" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="G157" s="4">
-        <v>1500</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="G157" s="4"/>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B158" s="2">
-        <v>100001600</v>
+        <v>120001605</v>
       </c>
       <c r="C158" s="3">
         <v>16</v>
       </c>
       <c r="D158" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E158" s="4">
-        <v>1600</v>
+        <v>1605</v>
       </c>
       <c r="F158" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="G158" s="4"/>
+      <c r="G158" s="4">
+        <v>1600</v>
+      </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B159" s="2">
-        <v>120001605</v>
+        <v>120101601</v>
       </c>
       <c r="C159" s="3">
         <v>16</v>
       </c>
       <c r="D159" s="3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E159" s="4">
-        <v>1605</v>
+        <v>1601</v>
       </c>
       <c r="F159" s="2" t="s">
         <v>176</v>
@@ -4630,19 +4627,19 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B160" s="2">
-        <v>120101601</v>
+        <v>120101602</v>
       </c>
       <c r="C160" s="3">
         <v>16</v>
       </c>
       <c r="D160" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E160" s="4">
-        <v>1601</v>
+        <v>1602</v>
       </c>
       <c r="F160" s="2" t="s">
         <v>177</v>
@@ -4653,19 +4650,19 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B161" s="2">
-        <v>120101602</v>
+        <v>120101603</v>
       </c>
       <c r="C161" s="3">
         <v>16</v>
       </c>
       <c r="D161" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E161" s="4">
-        <v>1602</v>
+        <v>1603</v>
       </c>
       <c r="F161" s="2" t="s">
         <v>178</v>
@@ -4676,19 +4673,19 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B162" s="2">
-        <v>120101603</v>
+        <v>120101604</v>
       </c>
       <c r="C162" s="3">
         <v>16</v>
       </c>
       <c r="D162" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E162" s="4">
-        <v>1603</v>
+        <v>1604</v>
       </c>
       <c r="F162" s="2" t="s">
         <v>179</v>
@@ -4699,19 +4696,19 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B163" s="2">
-        <v>120101604</v>
+        <v>121201606</v>
       </c>
       <c r="C163" s="3">
         <v>16</v>
       </c>
       <c r="D163" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E163" s="4">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="F163" s="2" t="s">
         <v>180</v>
@@ -4722,63 +4719,63 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="B164" s="2">
-        <v>121201606</v>
+        <v>100001700</v>
       </c>
       <c r="C164" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D164" s="3">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E164" s="4">
-        <v>1606</v>
+        <v>1700</v>
       </c>
       <c r="F164" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="G164" s="4">
-        <v>1600</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="G164" s="4"/>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B165" s="2">
-        <v>100001700</v>
+        <v>123001718</v>
       </c>
       <c r="C165" s="3">
         <v>17</v>
       </c>
       <c r="D165" s="3">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="E165" s="4">
-        <v>1700</v>
+        <v>1718</v>
       </c>
       <c r="F165" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="G165" s="4"/>
+      <c r="G165" s="4">
+        <v>1700</v>
+      </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B166" s="2">
-        <v>123001718</v>
+        <v>137001720</v>
       </c>
       <c r="C166" s="3">
         <v>17</v>
       </c>
       <c r="D166" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E166" s="4">
-        <v>1718</v>
+        <v>1720</v>
       </c>
       <c r="F166" s="2" t="s">
         <v>184</v>
@@ -4789,19 +4786,19 @@
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B167" s="2">
-        <v>137001720</v>
+        <v>140001702</v>
       </c>
       <c r="C167" s="3">
         <v>17</v>
       </c>
       <c r="D167" s="3">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E167" s="4">
-        <v>1720</v>
+        <v>1702</v>
       </c>
       <c r="F167" s="2" t="s">
         <v>185</v>
@@ -4812,19 +4809,19 @@
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B168" s="2">
-        <v>140001702</v>
+        <v>140001703</v>
       </c>
       <c r="C168" s="3">
         <v>17</v>
       </c>
       <c r="D168" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E168" s="4">
-        <v>1702</v>
+        <v>1703</v>
       </c>
       <c r="F168" s="2" t="s">
         <v>186</v>
@@ -4835,19 +4832,19 @@
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B169" s="2">
-        <v>140001703</v>
+        <v>141001704</v>
       </c>
       <c r="C169" s="3">
         <v>17</v>
       </c>
       <c r="D169" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E169" s="4">
-        <v>1703</v>
+        <v>1704</v>
       </c>
       <c r="F169" s="2" t="s">
         <v>187</v>
@@ -4858,19 +4855,19 @@
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B170" s="2">
-        <v>141001704</v>
+        <v>141001705</v>
       </c>
       <c r="C170" s="3">
         <v>17</v>
       </c>
       <c r="D170" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E170" s="4">
-        <v>1704</v>
+        <v>1705</v>
       </c>
       <c r="F170" s="2" t="s">
         <v>188</v>
@@ -4881,19 +4878,19 @@
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B171" s="2">
-        <v>141001705</v>
+        <v>141001706</v>
       </c>
       <c r="C171" s="3">
         <v>17</v>
       </c>
       <c r="D171" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E171" s="4">
-        <v>1705</v>
+        <v>1706</v>
       </c>
       <c r="F171" s="2" t="s">
         <v>189</v>
@@ -4904,19 +4901,19 @@
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B172" s="2">
-        <v>141001706</v>
+        <v>141001707</v>
       </c>
       <c r="C172" s="3">
         <v>17</v>
       </c>
       <c r="D172" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E172" s="4">
-        <v>1706</v>
+        <v>1707</v>
       </c>
       <c r="F172" s="2" t="s">
         <v>190</v>
@@ -4927,19 +4924,19 @@
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B173" s="2">
-        <v>141001707</v>
+        <v>150001708</v>
       </c>
       <c r="C173" s="3">
         <v>17</v>
       </c>
       <c r="D173" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E173" s="4">
-        <v>1707</v>
+        <v>1708</v>
       </c>
       <c r="F173" s="2" t="s">
         <v>191</v>
@@ -4950,19 +4947,19 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B174" s="2">
-        <v>150001708</v>
+        <v>150001709</v>
       </c>
       <c r="C174" s="3">
         <v>17</v>
       </c>
       <c r="D174" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E174" s="4">
-        <v>1708</v>
+        <v>1709</v>
       </c>
       <c r="F174" s="2" t="s">
         <v>192</v>
@@ -4973,19 +4970,19 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B175" s="2">
-        <v>150001709</v>
+        <v>150001710</v>
       </c>
       <c r="C175" s="3">
         <v>17</v>
       </c>
       <c r="D175" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E175" s="4">
-        <v>1709</v>
+        <v>1710</v>
       </c>
       <c r="F175" s="2" t="s">
         <v>193</v>
@@ -4996,19 +4993,19 @@
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B176" s="2">
-        <v>150001710</v>
+        <v>150001711</v>
       </c>
       <c r="C176" s="3">
         <v>17</v>
       </c>
       <c r="D176" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E176" s="4">
-        <v>1710</v>
+        <v>1711</v>
       </c>
       <c r="F176" s="2" t="s">
         <v>194</v>
@@ -5019,19 +5016,19 @@
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B177" s="2">
-        <v>150001711</v>
+        <v>150001712</v>
       </c>
       <c r="C177" s="3">
         <v>17</v>
       </c>
       <c r="D177" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E177" s="4">
-        <v>1711</v>
+        <v>1712</v>
       </c>
       <c r="F177" s="2" t="s">
         <v>195</v>
@@ -5042,19 +5039,19 @@
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B178" s="2">
-        <v>150001712</v>
+        <v>150001713</v>
       </c>
       <c r="C178" s="3">
         <v>17</v>
       </c>
       <c r="D178" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E178" s="4">
-        <v>1712</v>
+        <v>1713</v>
       </c>
       <c r="F178" s="2" t="s">
         <v>196</v>
@@ -5065,19 +5062,19 @@
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B179" s="2">
-        <v>150001713</v>
+        <v>150001714</v>
       </c>
       <c r="C179" s="3">
         <v>17</v>
       </c>
       <c r="D179" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E179" s="4">
-        <v>1713</v>
+        <v>1714</v>
       </c>
       <c r="F179" s="2" t="s">
         <v>197</v>
@@ -5088,19 +5085,19 @@
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B180" s="2">
-        <v>150001714</v>
+        <v>150001715</v>
       </c>
       <c r="C180" s="3">
         <v>17</v>
       </c>
       <c r="D180" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E180" s="4">
-        <v>1714</v>
+        <v>1715</v>
       </c>
       <c r="F180" s="2" t="s">
         <v>198</v>
@@ -5111,19 +5108,19 @@
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B181" s="2">
-        <v>150001715</v>
+        <v>150001716</v>
       </c>
       <c r="C181" s="3">
         <v>17</v>
       </c>
       <c r="D181" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E181" s="4">
-        <v>1715</v>
+        <v>1716</v>
       </c>
       <c r="F181" s="2" t="s">
         <v>199</v>
@@ -5134,19 +5131,19 @@
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B182" s="2">
-        <v>150001716</v>
+        <v>150001717</v>
       </c>
       <c r="C182" s="3">
         <v>17</v>
       </c>
       <c r="D182" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E182" s="4">
-        <v>1716</v>
+        <v>1717</v>
       </c>
       <c r="F182" s="2" t="s">
         <v>200</v>
@@ -5157,19 +5154,19 @@
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B183" s="2">
-        <v>150001717</v>
+        <v>153001701</v>
       </c>
       <c r="C183" s="3">
         <v>17</v>
       </c>
       <c r="D183" s="3">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E183" s="4">
-        <v>1717</v>
+        <v>1701</v>
       </c>
       <c r="F183" s="2" t="s">
         <v>201</v>
@@ -5180,47 +5177,24 @@
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B184" s="2">
-        <v>153001701</v>
+        <v>168001719</v>
       </c>
       <c r="C184" s="3">
         <v>17</v>
       </c>
       <c r="D184" s="3">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="E184" s="4">
-        <v>1701</v>
+        <v>1719</v>
       </c>
       <c r="F184" s="2" t="s">
         <v>202</v>
       </c>
       <c r="G184" s="4">
-        <v>1700</v>
-      </c>
-    </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A185" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="B185" s="2">
-        <v>168001719</v>
-      </c>
-      <c r="C185" s="3">
-        <v>17</v>
-      </c>
-      <c r="D185" s="3">
-        <v>19</v>
-      </c>
-      <c r="E185" s="4">
-        <v>1719</v>
-      </c>
-      <c r="F185" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="G185" s="4">
         <v>1700</v>
       </c>
     </row>

</xml_diff>